<commit_message>
update cv to new courses
</commit_message>
<xml_diff>
--- a/count_students.xlsx
+++ b/count_students.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB56D5C-5CF3-4D6E-BFB8-C3D9B2D23671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8540390F-BCB5-49DC-966B-CF76F5E3D751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{152D85A7-6ADB-4D3D-9731-2BD3ABA9C500}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{152D85A7-6ADB-4D3D-9731-2BD3ABA9C500}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="28">
   <si>
     <t>שנה</t>
   </si>
@@ -494,25 +494,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA99827-F5F0-41BD-81FC-680D1AE82FB7}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,15 +538,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -555,76 +555,79 @@
         <v>6</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -650,7 +653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -673,50 +676,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
       </c>
       <c r="F8">
-        <v>50</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -736,15 +736,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -753,18 +753,18 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -773,12 +773,12 @@
         <v>6</v>
       </c>
       <c r="F12">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -793,18 +793,18 @@
         <v>6</v>
       </c>
       <c r="F13">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -813,10 +813,10 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -836,215 +836,212 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>2023</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2024</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2025</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2023</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2024</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2026</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2018</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>2022</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2022</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2022</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2022</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2022</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24">
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>2023</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2023</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2023</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2023</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>2024</v>
       </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2023</v>
-      </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1053,18 +1050,21 @@
         <v>9</v>
       </c>
       <c r="F26">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2023</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1073,32 +1073,32 @@
         <v>9</v>
       </c>
       <c r="F27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2023</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
       </c>
       <c r="F28">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1113,15 +1113,15 @@
         <v>9</v>
       </c>
       <c r="F29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1133,10 +1133,10 @@
         <v>9</v>
       </c>
       <c r="F30">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2024</v>
       </c>
@@ -1144,67 +1144,64 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
       </c>
       <c r="F31">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32">
         <v>13</v>
       </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
-      <c r="F33">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2024</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -1213,55 +1210,52 @@
         <v>9</v>
       </c>
       <c r="F34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2024</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="H35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
       </c>
       <c r="F36">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -1270,21 +1264,21 @@
         <v>13</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
       </c>
       <c r="F37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
@@ -1296,18 +1290,18 @@
         <v>9</v>
       </c>
       <c r="F38">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1316,35 +1310,35 @@
         <v>9</v>
       </c>
       <c r="F39">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
       </c>
       <c r="F40">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2025</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -1356,33 +1350,158 @@
         <v>9</v>
       </c>
       <c r="F41">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2025</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="s">
         <v>9</v>
       </c>
       <c r="F42">
-        <v>103</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2024</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2026</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2026</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2026</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2026</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2026</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H42" xr:uid="{2DA99827-F5F0-41BD-81FC-680D1AE82FB7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:H39">
-      <sortCondition ref="C1:C42"/>
+  <autoFilter ref="A1:H49" xr:uid="{2DA99827-F5F0-41BD-81FC-680D1AE82FB7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H15">
+      <sortCondition ref="D1:D49"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>